<commit_message>
In progress refactoring and Unit Testing of Manager Controller.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Pipe/Rattle</t>
   </si>
   <si>
-    <t>House Hunting Backlog</t>
-  </si>
-  <si>
     <t>Storage Architecture for Media</t>
   </si>
   <si>
@@ -247,13 +244,19 @@
     <t>CD Storage</t>
   </si>
   <si>
-    <t>Tax Accountants on SATURDAY 9/8</t>
-  </si>
-  <si>
     <t>T-Shirts (get them!), Jeans, Kicks</t>
   </si>
   <si>
     <t>Goto the Doctor and get checked up - Call Kachar</t>
+  </si>
+  <si>
+    <t>Write check for $3600 to State of IL</t>
+  </si>
+  <si>
+    <t>TUESDAY 9/11</t>
+  </si>
+  <si>
+    <t>Download and start using YNAB</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -721,7 +726,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -729,7 +734,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>0</v>
@@ -743,15 +748,15 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="18" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>40</v>
@@ -759,18 +764,18 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="18" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>0</v>
+      <c r="A14" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -788,7 +793,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>0</v>
@@ -796,7 +801,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>40</v>
@@ -825,17 +830,17 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -855,7 +860,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -868,7 +873,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>40</v>
@@ -876,12 +881,12 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>40</v>
@@ -889,7 +894,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>40</v>
@@ -918,13 +923,13 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1091,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1102,7 +1107,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1113,7 +1118,7 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1124,7 +1129,7 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
Baby-step on finishing the QfHtmlHelpers
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -245,15 +245,6 @@
   </si>
   <si>
     <t>T-Shirts (get them!), Jeans, Kicks</t>
-  </si>
-  <si>
-    <t>Goto the Doctor and get checked up - Call Kachar</t>
-  </si>
-  <si>
-    <t>Write check for $3600 to State of IL</t>
-  </si>
-  <si>
-    <t>TUESDAY 9/11</t>
   </si>
   <si>
     <t>Download and start using YNAB</t>
@@ -682,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A11" sqref="A11:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,62 +739,46 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="18" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>40</v>
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="14" t="s">
+      <c r="A17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B17" s="13" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Saving my precious notes!
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Project Ingrid - Insurance Calculator</t>
   </si>
   <si>
-    <t>Generic Backlog</t>
-  </si>
-  <si>
     <t>Professional</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>New Honda Problem List</t>
   </si>
   <si>
-    <t>Read the ACIM Text</t>
-  </si>
-  <si>
     <t>Window Chip</t>
   </si>
   <si>
@@ -202,9 +196,6 @@
     <t>Find Invoicing Software</t>
   </si>
   <si>
-    <t>Pleiades (MVC + C# + Git + JavaScript + Azure)</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -220,9 +211,6 @@
     <t>Buy Resharper</t>
   </si>
   <si>
-    <t>Bank of America Maintenance Fees</t>
-  </si>
-  <si>
     <t>LOL</t>
   </si>
   <si>
@@ -248,6 +236,21 @@
   </si>
   <si>
     <t>Download and start using YNAB</t>
+  </si>
+  <si>
+    <t>Perform Daily Workbook Exercise</t>
+  </si>
+  <si>
+    <t>Finish E-Trade, Verizon, benefits</t>
+  </si>
+  <si>
+    <t>Bank of America Maintenance Fees -- Account Fee</t>
+  </si>
+  <si>
+    <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure)</t>
+  </si>
+  <si>
+    <t>All-in-All Backlog</t>
   </si>
 </sst>
 </file>
@@ -343,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -377,6 +380,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -673,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -689,7 +696,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="15" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -697,89 +704,105 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6"/>
+    <row r="5" spans="1:2">
+      <c r="A5" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>0</v>
-      </c>
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10"/>
+    <row r="9" spans="1:2">
+      <c r="A9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>40</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="18" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>40</v>
+      <c r="A13" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="A15" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>40</v>
+    <row r="19" spans="1:2">
+      <c r="A19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -805,74 +828,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="20" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -898,13 +921,13 @@
   <sheetData>
     <row r="3" spans="1:3">
       <c r="A3" s="17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1060,75 +1083,75 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1151,52 +1174,52 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1222,42 +1245,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -1277,17 +1300,17 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1310,42 +1333,42 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Category Editor in progress.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -238,9 +238,6 @@
     <t>Perform Daily Workbook Exercise</t>
   </si>
   <si>
-    <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure)</t>
-  </si>
-  <si>
     <t>All-in-All Backlog</t>
   </si>
   <si>
@@ -250,34 +247,16 @@
     <t>Brush up Resume and get Linked-in on full blast</t>
   </si>
   <si>
-    <t>Focus on mastering Game w/ Redbox</t>
-  </si>
-  <si>
-    <t>What happened to my Paycheck AND Fidelity…?</t>
-  </si>
-  <si>
-    <t>MONDAY</t>
-  </si>
-  <si>
-    <t>Verizon Reimbursment - Ask for a Receipt from Gracie</t>
-  </si>
-  <si>
-    <t>Create Househunting Requirements</t>
-  </si>
-  <si>
     <t>Finish Clearing Email - Give Yelp and Order  Gracie Mag</t>
   </si>
   <si>
-    <t>Paper Sort</t>
-  </si>
-  <si>
-    <t>TUESDAY</t>
-  </si>
-  <si>
-    <t>Branding Plan</t>
-  </si>
-  <si>
-    <t>Get back to Matty</t>
+    <t>Verizon Reimbursment + Submit Receipt from Gracie</t>
+  </si>
+  <si>
+    <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + Sammy)</t>
+  </si>
+  <si>
+    <t>Invoice DC Export</t>
   </si>
 </sst>
 </file>
@@ -323,7 +302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +339,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -373,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -406,11 +391,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -707,15 +697,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="62.42578125" customWidth="1"/>
+    <col min="1" max="1" width="74.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
@@ -723,7 +713,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -744,10 +734,10 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>39</v>
       </c>
     </row>
@@ -759,7 +749,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>0</v>
@@ -767,124 +757,76 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="23" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B16" s="27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="14" t="s">
+      <c r="A20" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Amazing - proof of concept very much, well underway.  Good job, Aleks!
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -9,18 +9,16 @@
   <sheets>
     <sheet name="Generic Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Shopping List" sheetId="6" r:id="rId2"/>
-    <sheet name="SCIGON Payroll Summary" sheetId="15" r:id="rId3"/>
-    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId4"/>
-    <sheet name="New Honda Problems" sheetId="14" r:id="rId5"/>
-    <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId6"/>
-    <sheet name="Hosts" sheetId="9" r:id="rId7"/>
+    <sheet name="Try, Do, Explore" sheetId="8" r:id="rId3"/>
+    <sheet name="New Honda Problems" sheetId="14" r:id="rId4"/>
+    <sheet name="Services, Markets &amp; Ideas" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -82,9 +80,6 @@
     <t>Social Assassin / Game</t>
   </si>
   <si>
-    <t>Born Bolt</t>
-  </si>
-  <si>
     <t>Shared Hosting =&gt; http://discountasp.net</t>
   </si>
   <si>
@@ -196,15 +191,6 @@
     <t>Find Invoicing Software</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
     <t>Buy Student Edition Photoshop</t>
   </si>
   <si>
@@ -244,19 +230,22 @@
     <t>Jeans and new Casual Shoes</t>
   </si>
   <si>
-    <t>Brush up Resume and get Linked-in on full blast</t>
-  </si>
-  <si>
-    <t>Finish Clearing Email - Give Yelp and Order  Gracie Mag</t>
-  </si>
-  <si>
     <t>Verizon Reimbursment + Submit Receipt from Gracie</t>
   </si>
   <si>
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + Sammy)</t>
   </si>
   <si>
-    <t>Invoice DC Export</t>
+    <t>Linked-in on full blast</t>
+  </si>
+  <si>
+    <t>Brush up Resume</t>
+  </si>
+  <si>
+    <t>Give Yelp and Order  Gracie Mag</t>
+  </si>
+  <si>
+    <t>Another pair of Glasses</t>
   </si>
 </sst>
 </file>
@@ -302,7 +291,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,12 +313,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -358,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -372,23 +355,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -399,10 +373,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,8 +687,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
-      <c r="A1" s="15" t="s">
-        <v>72</v>
+      <c r="A1" s="12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -726,19 +701,19 @@
       <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>39</v>
+      <c r="A5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -748,35 +723,35 @@
       <c r="B7"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>0</v>
+      <c r="A9" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>39</v>
+      <c r="A10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>39</v>
+      <c r="A11" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -786,48 +761,56 @@
       <c r="B13"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>39</v>
+      <c r="A15" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
+      <c r="A16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>39</v>
+    <row r="21" spans="1:2">
+      <c r="A21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -838,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A8" sqref="A8:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,74 +836,69 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>67</v>
+      <c r="A9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>39</v>
+      <c r="A10" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>64</v>
+      <c r="A13" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>39</v>
+      <c r="A14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -930,169 +908,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:3">
-      <c r="A3" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="16">
-        <v>40931</v>
-      </c>
-      <c r="B4" s="16">
-        <v>40944</v>
-      </c>
-      <c r="C4">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="16">
-        <v>40945</v>
-      </c>
-      <c r="B5" s="16">
-        <v>40958</v>
-      </c>
-      <c r="C5">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="16">
-        <v>40959</v>
-      </c>
-      <c r="B6" s="16">
-        <v>40972</v>
-      </c>
-      <c r="C6">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="16">
-        <v>40973</v>
-      </c>
-      <c r="B7" s="16">
-        <v>40986</v>
-      </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="16">
-        <v>40987</v>
-      </c>
-      <c r="B8" s="16">
-        <v>41000</v>
-      </c>
-      <c r="C8">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="16">
-        <v>41001</v>
-      </c>
-      <c r="B9" s="16">
-        <v>41014</v>
-      </c>
-      <c r="C9">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="16">
-        <v>41015</v>
-      </c>
-      <c r="B10" s="16">
-        <v>41028</v>
-      </c>
-      <c r="C10">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="16">
-        <v>41029</v>
-      </c>
-      <c r="B11" s="16">
-        <v>41042</v>
-      </c>
-      <c r="C11">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="16">
-        <v>41043</v>
-      </c>
-      <c r="B12" s="16">
-        <v>41056</v>
-      </c>
-      <c r="C12">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="16">
-        <v>41057</v>
-      </c>
-      <c r="B13" s="16">
-        <v>41070</v>
-      </c>
-      <c r="C13">
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="16">
-        <v>41071</v>
-      </c>
-      <c r="B14" s="16">
-        <v>41084</v>
-      </c>
-      <c r="C14">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="16">
-        <v>41085</v>
-      </c>
-      <c r="B15" s="16">
-        <v>41098</v>
-      </c>
-      <c r="C15">
-        <v>77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1113,13 +928,13 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1127,10 +942,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1138,10 +953,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1152,7 +967,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1160,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1176,7 +991,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -1198,53 +1013,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="12" t="s">
-        <v>42</v>
+      <c r="A1" s="11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1253,12 +1068,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A16"/>
+      <selection activeCell="A19" sqref="A19:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1269,28 +1084,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="12" t="s">
-        <v>35</v>
+      <c r="A1" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="4" t="s">
-        <v>34</v>
+      <c r="A5" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1">
@@ -1300,12 +1115,12 @@
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:1">
@@ -1330,74 +1145,55 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="23.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="57.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="23.25">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Unprecedented refactoring and recovery, due to good design, solid testing and so forth.  Good job, Aleks.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Jeans and new Casual Shoes + Jacket!</t>
+  </si>
+  <si>
+    <t>Find a forum for Personal Finance /  Questions about  Mortgage</t>
   </si>
 </sst>
 </file>
@@ -672,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -762,54 +765,62 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B16" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="19" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B17" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="23" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="17" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="21" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="23" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduction of the Unit of Work pattern, rewiring of the Membership Repository Factory, fix to SecurityAttribute dependency resolution
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -227,15 +227,9 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + Sammy)</t>
-  </si>
-  <si>
     <t>Linked-in on full blast</t>
   </si>
   <si>
-    <t>Brush up Resume</t>
-  </si>
-  <si>
     <t>Give Yelp and Order  Gracie Mag</t>
   </si>
   <si>
@@ -245,10 +239,19 @@
     <t>Verizon Reimbursment</t>
   </si>
   <si>
-    <t>Find a forum for Personal Finance /  Questions about  Mortgage</t>
-  </si>
-  <si>
     <t>Jeans and new Casual Shoes</t>
+  </si>
+  <si>
+    <t>House Hunting  Backlog</t>
+  </si>
+  <si>
+    <t>Bradley Method Book</t>
+  </si>
+  <si>
+    <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
+  </si>
+  <si>
+    <t>Check-up on Git / Change Password for security</t>
   </si>
 </sst>
 </file>
@@ -675,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,64 +715,64 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B6" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="13" t="s">
+      <c r="B8"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="20" t="s">
+      <c r="B12" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>38</v>
-      </c>
+      <c r="B14"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="13" t="s">
@@ -781,46 +784,54 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="B22" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="21" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B23" s="23" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mid-stream with developing Categories data layer.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -251,7 +251,7 @@
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
   </si>
   <si>
-    <t>Check-up on Git / Change Password for security</t>
+    <t>New ToastMasters speech</t>
   </si>
 </sst>
 </file>
@@ -681,7 +681,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
MILESTONE: integration of the full Category editing w/ persistence.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -347,15 +347,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -364,26 +361,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,52 +684,48 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="75" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="77.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="19" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3"/>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -734,37 +733,36 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -772,45 +770,44 @@
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14"/>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -820,18 +817,18 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="21" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -887,18 +884,18 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -908,18 +905,18 @@
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -940,7 +937,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="23.25">
@@ -949,10 +946,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
@@ -963,7 +960,7 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
@@ -974,7 +971,7 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C5" t="s">
@@ -985,7 +982,7 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
@@ -996,7 +993,7 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1004,7 +1001,7 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1012,7 +1009,7 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1035,7 +1032,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1106,7 +1103,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1116,7 +1113,7 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Massive update with introduction of numerous Domain objects
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t>Buy Student Edition Photoshop</t>
-  </si>
-  <si>
-    <t>Buy Resharper</t>
   </si>
   <si>
     <t>LOL</t>
@@ -681,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A10" sqref="A10:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -697,7 +694,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -707,7 +704,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>0</v>
@@ -715,7 +712,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>0</v>
@@ -736,99 +733,91 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="20" t="s">
+      <c r="A10" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="17" t="s">
+      <c r="A22" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B22" s="24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -855,17 +844,17 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -880,7 +869,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -893,7 +882,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>38</v>
@@ -901,7 +890,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -953,7 +942,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -964,7 +953,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -975,7 +964,7 @@
         <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -986,7 +975,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
Exceptional!  Created the back-end for storing files, images and the like (Resources).
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>House Hunting  Backlog</t>
-  </si>
-  <si>
-    <t>Bradley Method Book</t>
   </si>
   <si>
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
@@ -678,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B22"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -710,114 +707,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="12" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B7" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="15" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B16" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="20" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="17" t="s">
+      <c r="A21" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B21" s="24" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
File Resource Upload stuff.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -224,12 +224,6 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Linked-in on full blast</t>
-  </si>
-  <si>
-    <t>Give Yelp and Order  Gracie Mag</t>
-  </si>
-  <si>
     <t>Another pair of Glasses</t>
   </si>
   <si>
@@ -246,13 +240,19 @@
   </si>
   <si>
     <t>New ToastMasters speech</t>
+  </si>
+  <si>
+    <t>SATURDAY?</t>
+  </si>
+  <si>
+    <t>Linked-in =&gt; add everybody from the Red Poole</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +289,14 @@
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -362,7 +370,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -379,6 +386,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -675,16 +685,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="77.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="19" customWidth="1"/>
+    <col min="1" max="1" width="79.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="18" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
@@ -703,7 +713,7 @@
       <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
     </row>
@@ -714,25 +724,25 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -740,36 +750,37 @@
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>38</v>
+      <c r="A14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -777,36 +788,28 @@
       <c r="A16" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>38</v>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>52</v>
+      <c r="A19" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="17" t="s">
+      <c r="A20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rapid development - added the Color Editor
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>3 PM Saturday</t>
+  </si>
+  <si>
+    <t>Organize my Contacts Database</t>
+  </si>
+  <si>
+    <t>FOLLOW-UP  ON REDBOX EMAIL</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
   </si>
 </sst>
 </file>
@@ -352,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -371,7 +380,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -392,6 +400,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -688,16 +701,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
@@ -716,7 +729,7 @@
       <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -729,7 +742,7 @@
       <c r="A7" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>0</v>
       </c>
     </row>
@@ -737,82 +750,90 @@
       <c r="A8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>0</v>
-      </c>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="16" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B16" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="15" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="17" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Product List View in progress.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -224,9 +224,6 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Another pair of Glasses</t>
-  </si>
-  <si>
     <t>Verizon Reimbursment</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
   </si>
   <si>
     <t>Linked-in =&gt; add everybody from the Red Poole</t>
-  </si>
-  <si>
-    <t>3 PM Saturday</t>
   </si>
   <si>
     <t>Organize my Contacts Database</t>
@@ -701,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,7 +734,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -748,15 +742,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>38</v>
@@ -764,7 +758,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>38</v>
@@ -778,7 +772,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>0</v>
@@ -786,54 +780,46 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>52</v>
+      <c r="B19" s="19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="16" t="s">
+      <c r="A20" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completion of Product Editor Refactoring
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -224,9 +224,6 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Verizon Reimbursment</t>
-  </si>
-  <si>
     <t>Jeans and new Casual Shoes</t>
   </si>
   <si>
@@ -236,22 +233,13 @@
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
   </si>
   <si>
-    <t>New ToastMasters speech</t>
-  </si>
-  <si>
     <t>SATURDAY?</t>
   </si>
   <si>
-    <t>Linked-in =&gt; add everybody from the Red Poole</t>
-  </si>
-  <si>
     <t>Organize my Contacts Database</t>
   </si>
   <si>
-    <t>FOLLOW-UP  ON REDBOX EMAIL</t>
-  </si>
-  <si>
-    <t>SUNDAY</t>
+    <t>Linked-in =&gt; add everybody from the Red Poole (add Alyssa Liddle)</t>
   </si>
 </sst>
 </file>
@@ -355,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -397,10 +385,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,16 +680,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="79.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="17" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
@@ -734,7 +719,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -742,84 +727,68 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="21" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="18" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="16" t="s">
+      <c r="A18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Back in the DDD realm
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -224,9 +224,6 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Jeans and new Casual Shoes</t>
-  </si>
-  <si>
     <t>House Hunting  Backlog</t>
   </si>
   <si>
@@ -240,6 +237,18 @@
   </si>
   <si>
     <t>Linked-in =&gt; add everybody from the Red Poole (add Alyssa Liddle)</t>
+  </si>
+  <si>
+    <t>Pimp Jeans and new Casual Shoes</t>
+  </si>
+  <si>
+    <t>Exchange that Shitty Printer</t>
+  </si>
+  <si>
+    <t>Jeff, Keith, Phil, Andy, Omar, Brad</t>
+  </si>
+  <si>
+    <t>WHENEVS</t>
   </si>
 </sst>
 </file>
@@ -680,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -719,7 +728,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -727,68 +736,84 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="23"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="18" t="s">
+      <c r="B19" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="16" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleared some technical debts with the Image Bundle Viewer
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -224,9 +224,6 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>House Hunting  Backlog</t>
-  </si>
-  <si>
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
   </si>
   <si>
@@ -245,10 +242,10 @@
     <t>Exchange that Shitty Printer</t>
   </si>
   <si>
-    <t>Jeff, Keith, Phil, Andy, Omar, Brad</t>
-  </si>
-  <si>
     <t>WHENEVS</t>
+  </si>
+  <si>
+    <t>Jeff, Keith, Phil, Andy, Brad, Andrei</t>
   </si>
 </sst>
 </file>
@@ -689,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,7 +725,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
@@ -736,18 +733,18 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -755,12 +752,12 @@
         <v>75</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>38</v>
@@ -773,47 +770,39 @@
       <c r="B13" s="23"/>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="16" t="s">
+      <c r="A19" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B19" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pounding away.  Stick with it, son!
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -227,25 +227,16 @@
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
   </si>
   <si>
-    <t>SATURDAY?</t>
-  </si>
-  <si>
-    <t>Organize my Contacts Database</t>
-  </si>
-  <si>
     <t>Linked-in =&gt; add everybody from the Red Poole (add Alyssa Liddle)</t>
   </si>
   <si>
     <t>Pimp Jeans and new Casual Shoes</t>
   </si>
   <si>
-    <t>Exchange that Shitty Printer</t>
-  </si>
-  <si>
-    <t>WHENEVS</t>
-  </si>
-  <si>
-    <t>Jeff, Keith, Phil, Andy, Brad, Andrei, Ajit, Ryan</t>
+    <t>Connect with Marc Johnson</t>
+  </si>
+  <si>
+    <t>Jeff Benson, Organize my Contacts Database =&gt;  Keith, Phil, Andy, Brad, Andrei, Ajit, Ryan</t>
   </si>
 </sst>
 </file>
@@ -686,31 +677,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="79.28515625" customWidth="1"/>
+    <col min="1" max="1" width="87.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="17" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25">
+    <row r="1" spans="1:3" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
@@ -718,12 +709,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="12" t="s">
         <v>68</v>
       </c>
@@ -731,45 +722,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" s="20" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
+      <c r="C10" s="17"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="25" t="s">
         <v>51</v>
       </c>
@@ -777,32 +769,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>38</v>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>52</v>
+      <c r="A17" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="16" t="s">
+      <c r="A18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B18" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continued leaps and bounds.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="74">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Pleiades (MVC + C# + Git + Bootstrap + Jquery + Knockout + Azure + EF + JavaScript)</t>
   </si>
   <si>
-    <t>Linked-in =&gt; add everybody from the Red Poole (add Alyssa Liddle)</t>
-  </si>
-  <si>
     <t>Pimp Jeans and new Casual Shoes</t>
   </si>
   <si>
@@ -237,13 +234,19 @@
   </si>
   <si>
     <t>Jeff Benson, Organize my Contacts Database =&gt;  Keith, Phil, Andy, Brad, Andrei, Ajit, Ryan</t>
+  </si>
+  <si>
+    <t>http://www.webroot.com/En_US/sites/aff-wsc-29/?ref=cj&amp;rc=2614</t>
+  </si>
+  <si>
+    <t>Linked-in =&gt; add everybody from the Red Poole</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +291,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -337,10 +347,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,8 +397,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -691,17 +708,17 @@
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
@@ -709,90 +726,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="26"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4">
+      <c r="A9" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B11" s="21" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="21" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="23"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="18" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="20" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Upgrade to MVC 4 / EF5
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -221,34 +221,34 @@
     <t>All-in-All Backlog</t>
   </si>
   <si>
-    <t>Repair my Jeans and new Casual Shoes</t>
-  </si>
-  <si>
-    <t>Repair the Machine (Massage, Kachar, Chiro, Acupunture, ???)</t>
-  </si>
-  <si>
-    <t>Push Market</t>
-  </si>
-  <si>
     <t>Get Web Root Antivirus</t>
   </si>
   <si>
-    <t>Invoice Dominick</t>
-  </si>
-  <si>
     <t>Invoice Michael</t>
   </si>
   <si>
     <t>Use YNAB</t>
   </si>
   <si>
-    <t>Contact Fran</t>
-  </si>
-  <si>
-    <t>Cancel RedboxInstant.net</t>
-  </si>
-  <si>
     <t>Replacement Phone</t>
+  </si>
+  <si>
+    <t>Push Market (Phase 2)</t>
+  </si>
+  <si>
+    <t>New T-Shirts and Shoes</t>
+  </si>
+  <si>
+    <t>Haircut</t>
+  </si>
+  <si>
+    <t>Office + Machine 2.0</t>
+  </si>
+  <si>
+    <t>Marketing Escalation for Terminus 2.0</t>
+  </si>
+  <si>
+    <t>Repair the Machine = Ronnie + Acupuncture + PT</t>
   </si>
 </sst>
 </file>
@@ -309,7 +309,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,12 +342,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -369,7 +363,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,9 +387,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -404,15 +395,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -711,7 +697,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -734,7 +720,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="12" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>0</v>
@@ -752,19 +738,19 @@
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>0</v>
@@ -772,7 +758,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>0</v>
@@ -780,56 +766,56 @@
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="16" t="s">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="17" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="18"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="19"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="23" t="s">
-        <v>73</v>
+      <c r="A17" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -839,15 +825,15 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="18" t="s">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B22" s="22" t="s">

</xml_diff>

<commit_message>
Completed updating the Product Editor interface to use the new Glider library.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -236,10 +236,10 @@
     <t>Fofson (773) 603-9095, Clarence</t>
   </si>
   <si>
-    <t>Repair the Machine = Acupuncture?</t>
-  </si>
-  <si>
-    <t>Research and Upgrade =&gt; MAC</t>
+    <t>ALMOST DONE</t>
+  </si>
+  <si>
+    <t>Research and Upgrade =&gt; MAC + Win 8 + VS2013</t>
   </si>
 </sst>
 </file>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -715,91 +715,85 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="12" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="16" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="23" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="15"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="18"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="22" t="s">
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="21" t="s">
+      <c r="A17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B17" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Commerce Unit Tests, started building Membership Provider replacement.
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>New T-Shirts and Shoes</t>
-  </si>
-  <si>
-    <t>Fofson (773) 603-9095, Clarence</t>
   </si>
   <si>
     <t>ALMOST DONE</t>
@@ -354,7 +351,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,7 +390,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -689,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A14" sqref="A14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -737,10 +733,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -768,32 +764,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="22" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="21" t="s">
+      <c r="A16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B16" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another major namespace re-organization.  What can I say?
</commit_message>
<xml_diff>
--- a/Dev Notes/Personal/Master Backlog.xlsx
+++ b/Dev Notes/Personal/Master Backlog.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>IN PROGRESS</t>
   </si>
@@ -233,10 +233,10 @@
     <t>New T-Shirts and Shoes</t>
   </si>
   <si>
-    <t>ALMOST DONE</t>
-  </si>
-  <si>
     <t>Research and Upgrade =&gt; MAC + Win 8 + VS2013</t>
+  </si>
+  <si>
+    <t>Redbox - login to ADP, etc.</t>
   </si>
 </sst>
 </file>
@@ -685,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A7" sqref="A7:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -733,55 +733,61 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B10" s="23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
       <c r="C10" s="15"/>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="18"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="19" t="s">
+      <c r="B12" s="18"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B13" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B16" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="21" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B17" s="22" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>